<commit_message>
fixed the paths issues on report, screenshots and reading from excel
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cele\Documents\5thGroup\SauceDemo5thGroupBasicProject\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cele\Documents\GitProjects\SauceDemoAssessment\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B594E3-3EF1-455F-9776-508EADEA5484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00394A86-D87F-4B55-855E-AD807A957EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -35,40 +35,40 @@
     <t>Password</t>
   </si>
   <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Nkosingiphile</t>
+  </si>
+  <si>
+    <t>Cele</t>
+  </si>
+  <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Nkosingiphile</t>
-  </si>
-  <si>
-    <t>Cele</t>
   </si>
 </sst>
 </file>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,39 +451,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03AFC8B-6E56-45E6-B9B6-779FF57E859A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,21 +508,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>2094</v>

</xml_diff>

<commit_message>
Just pushing the latest code.
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cele\Documents\GitProjects\SauceDemoAssessment\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C817505\Documents\Personal Project\SauceDemoAssessment\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91961B5-67DE-4D2D-9E9B-4E9E6E8C7C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028BA6E5-6A5D-410B-AC3C-6D9EE5A5D51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -59,16 +59,19 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Nkosingiphile</t>
-  </si>
-  <si>
-    <t>Cele</t>
-  </si>
-  <si>
     <t>standard_user</t>
+  </si>
+  <si>
+    <t>Zamantuli</t>
+  </si>
+  <si>
+    <t>Xulu</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>1939</t>
   </si>
 </sst>
 </file>
@@ -143,12 +146,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,17 +435,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,39 +453,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -496,17 +500,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03AFC8B-6E56-45E6-B9B6-779FF57E859A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -514,27 +519,30 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3">
-        <v>2094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -546,7 +554,7 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>